<commit_message>
29-12-2017 : new form frmMastStatSec->Section used for portal release stratagy, and Bug Fixed : all bulk upload it selects temp filtered sheet ->removed, New SecCode is added in employee job profile
</commit_message>
<xml_diff>
--- a/upload_template/ShiftSchedule_Upload.xlsx
+++ b/upload_template/ShiftSchedule_Upload.xlsx
@@ -502,7 +502,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AG10" sqref="AG10"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +613,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>20005890</v>
+        <v>20010960</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
02-01-2017 : Some Enhensment as per user request, also Grace Period included
</commit_message>
<xml_diff>
--- a/upload_template/ShiftSchedule_Upload.xlsx
+++ b/upload_template/ShiftSchedule_Upload.xlsx
@@ -499,10 +499,10 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,13 +613,13 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>20010960</v>
+        <v>20005312</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -628,85 +628,85 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="S2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="T2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="Z2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AA2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020-08-01 : Contract Master -> Rate of Commission Added
</commit_message>
<xml_diff>
--- a/upload_template/ShiftSchedule_Upload.xlsx
+++ b/upload_template/ShiftSchedule_Upload.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24290A4E-93D7-44E2-B114-1DB6891548C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,9 +23,6 @@
     <t>WO</t>
   </si>
   <si>
-    <t>GN</t>
-  </si>
-  <si>
     <t>D01</t>
   </si>
   <si>
@@ -119,12 +117,15 @@
   </si>
   <si>
     <t>EmpUnqID</t>
+  </si>
+  <si>
+    <t>G1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,13 +189,13 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2 2 3" xfId="2"/>
-    <cellStyle name="Normal 2 3" xfId="3"/>
-    <cellStyle name="Normal 2 4" xfId="4"/>
-    <cellStyle name="Normal 3" xfId="5"/>
-    <cellStyle name="Normal 4" xfId="6"/>
-    <cellStyle name="Normal 9" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 2 2 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 9" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -285,6 +286,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -320,6 +338,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -495,14 +530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,195 +550,195 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>20005312</v>
+        <v>102434</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>0</v>

</xml_diff>